<commit_message>
Ajout du numéro améli au profil PractitionerRole (#260)
* Ajout du numéro améli au profil PractitionerRole

* Define slicing rules for PractitionerRole.identifier

Added slicing rules for PractitionerRole.identifier.

* add numero AM

* Change identifier 'numeroAm' cardinality to 0..1 f3e78d1ffa3d75459a69612bbe2ff0a2c02868d4
</commit_message>
<xml_diff>
--- a/main/ig/StructureDefinition-fr-core-organization.xlsx
+++ b/main/ig/StructureDefinition-fr-core-organization.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5275" uniqueCount="607">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5275" uniqueCount="608">
   <si>
     <t>Property</t>
   </si>
@@ -57,7 +57,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2026-01-09T10:08:27+00:00</t>
+    <t>2026-01-12T10:02:26+00:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -912,7 +912,10 @@
     <t>idNatSt</t>
   </si>
   <si>
-    <t>Identifiant national de structure unique délivré par une autorité d'enregistrement tel que défini dans l'Annexe Transverse Source des données métier pour les professionnels et les structures.</t>
+    <t>Identifiant national de structure, à privilégier. L'idNatSt ne doit pas être construit, il peut être trouvé via l'API Annuaire Santé.</t>
+  </si>
+  <si>
+    <t>Identifiant national de structure unique délivré par une autorité d'enregistrement tel que défini dans l'Annexe Transverse Source des données métier pour les professionnels et les structures. L'idNatSt ne doit pas être construit, pour trouver l'identifiant d'une structure, il suffit de faire une requête via l'API Annuaire Santé. Il s'agit de l'identifiant national à privilégier.</t>
   </si>
   <si>
     <t>Organization.identifier:idNatSt.id</t>
@@ -5844,7 +5847,7 @@
         <v>287</v>
       </c>
       <c r="M32" t="s" s="2">
-        <v>220</v>
+        <v>288</v>
       </c>
       <c r="N32" s="2"/>
       <c r="O32" t="s" s="2">
@@ -5926,7 +5929,7 @@
     </row>
     <row r="33">
       <c r="A33" t="s" s="2">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="B33" t="s" s="2">
         <v>229</v>
@@ -6038,7 +6041,7 @@
     </row>
     <row r="34">
       <c r="A34" t="s" s="2">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="B34" t="s" s="2">
         <v>230</v>
@@ -6152,7 +6155,7 @@
     </row>
     <row r="35">
       <c r="A35" t="s" s="2">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="B35" t="s" s="2">
         <v>231</v>
@@ -6200,7 +6203,7 @@
         <v>78</v>
       </c>
       <c r="S35" t="s" s="2">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="T35" t="s" s="2">
         <v>78</v>
@@ -6266,7 +6269,7 @@
     </row>
     <row r="36">
       <c r="A36" t="s" s="2">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="B36" t="s" s="2">
         <v>240</v>
@@ -6314,7 +6317,7 @@
         <v>78</v>
       </c>
       <c r="S36" t="s" s="2">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="T36" t="s" s="2">
         <v>78</v>
@@ -6380,7 +6383,7 @@
     </row>
     <row r="37">
       <c r="A37" t="s" s="2">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="B37" t="s" s="2">
         <v>249</v>
@@ -6428,7 +6431,7 @@
         <v>78</v>
       </c>
       <c r="S37" t="s" s="2">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="T37" t="s" s="2">
         <v>254</v>
@@ -6496,7 +6499,7 @@
     </row>
     <row r="38">
       <c r="A38" t="s" s="2">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="B38" t="s" s="2">
         <v>259</v>
@@ -6525,10 +6528,10 @@
         <v>102</v>
       </c>
       <c r="L38" t="s" s="2">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="M38" t="s" s="2">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="N38" t="s" s="2">
         <v>262</v>
@@ -6610,7 +6613,7 @@
     </row>
     <row r="39">
       <c r="A39" t="s" s="2">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="B39" t="s" s="2">
         <v>268</v>
@@ -6722,7 +6725,7 @@
     </row>
     <row r="40">
       <c r="A40" t="s" s="2">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="B40" t="s" s="2">
         <v>276</v>
@@ -6836,13 +6839,13 @@
     </row>
     <row r="41">
       <c r="A41" t="s" s="2">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="B41" t="s" s="2">
         <v>217</v>
       </c>
       <c r="C41" t="s" s="2">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="D41" t="s" s="2">
         <v>78</v>
@@ -6867,7 +6870,7 @@
         <v>218</v>
       </c>
       <c r="L41" t="s" s="2">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="M41" t="s" s="2">
         <v>220</v>
@@ -6952,7 +6955,7 @@
     </row>
     <row r="42">
       <c r="A42" t="s" s="2">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="B42" t="s" s="2">
         <v>229</v>
@@ -7064,7 +7067,7 @@
     </row>
     <row r="43">
       <c r="A43" t="s" s="2">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="B43" t="s" s="2">
         <v>230</v>
@@ -7178,7 +7181,7 @@
     </row>
     <row r="44">
       <c r="A44" t="s" s="2">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="B44" t="s" s="2">
         <v>231</v>
@@ -7292,7 +7295,7 @@
     </row>
     <row r="45">
       <c r="A45" t="s" s="2">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="B45" t="s" s="2">
         <v>240</v>
@@ -7340,7 +7343,7 @@
         <v>78</v>
       </c>
       <c r="S45" t="s" s="2">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="T45" t="s" s="2">
         <v>78</v>
@@ -7406,7 +7409,7 @@
     </row>
     <row r="46">
       <c r="A46" t="s" s="2">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="B46" t="s" s="2">
         <v>249</v>
@@ -7454,7 +7457,7 @@
         <v>78</v>
       </c>
       <c r="S46" t="s" s="2">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="T46" t="s" s="2">
         <v>254</v>
@@ -7522,7 +7525,7 @@
     </row>
     <row r="47">
       <c r="A47" t="s" s="2">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="B47" t="s" s="2">
         <v>259</v>
@@ -7636,7 +7639,7 @@
     </row>
     <row r="48">
       <c r="A48" t="s" s="2">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="B48" t="s" s="2">
         <v>268</v>
@@ -7748,7 +7751,7 @@
     </row>
     <row r="49">
       <c r="A49" t="s" s="2">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="B49" t="s" s="2">
         <v>276</v>
@@ -7862,13 +7865,13 @@
     </row>
     <row r="50">
       <c r="A50" t="s" s="2">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="B50" t="s" s="2">
         <v>217</v>
       </c>
       <c r="C50" t="s" s="2">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="D50" t="s" s="2">
         <v>78</v>
@@ -7893,7 +7896,7 @@
         <v>218</v>
       </c>
       <c r="L50" t="s" s="2">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="M50" t="s" s="2">
         <v>220</v>
@@ -7978,7 +7981,7 @@
     </row>
     <row r="51">
       <c r="A51" t="s" s="2">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="B51" t="s" s="2">
         <v>229</v>
@@ -8090,7 +8093,7 @@
     </row>
     <row r="52">
       <c r="A52" t="s" s="2">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="B52" t="s" s="2">
         <v>230</v>
@@ -8204,7 +8207,7 @@
     </row>
     <row r="53">
       <c r="A53" t="s" s="2">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="B53" t="s" s="2">
         <v>231</v>
@@ -8318,7 +8321,7 @@
     </row>
     <row r="54">
       <c r="A54" t="s" s="2">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="B54" t="s" s="2">
         <v>240</v>
@@ -8366,7 +8369,7 @@
         <v>78</v>
       </c>
       <c r="S54" t="s" s="2">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="T54" t="s" s="2">
         <v>78</v>
@@ -8432,7 +8435,7 @@
     </row>
     <row r="55">
       <c r="A55" t="s" s="2">
-        <v>322</v>
+        <v>323</v>
       </c>
       <c r="B55" t="s" s="2">
         <v>249</v>
@@ -8480,7 +8483,7 @@
         <v>78</v>
       </c>
       <c r="S55" t="s" s="2">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="T55" t="s" s="2">
         <v>254</v>
@@ -8548,7 +8551,7 @@
     </row>
     <row r="56">
       <c r="A56" t="s" s="2">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="B56" t="s" s="2">
         <v>259</v>
@@ -8662,7 +8665,7 @@
     </row>
     <row r="57">
       <c r="A57" t="s" s="2">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="B57" t="s" s="2">
         <v>268</v>
@@ -8774,7 +8777,7 @@
     </row>
     <row r="58">
       <c r="A58" t="s" s="2">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="B58" t="s" s="2">
         <v>276</v>
@@ -8888,13 +8891,13 @@
     </row>
     <row r="59">
       <c r="A59" t="s" s="2">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="B59" t="s" s="2">
         <v>217</v>
       </c>
       <c r="C59" t="s" s="2">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="D59" t="s" s="2">
         <v>78</v>
@@ -8919,7 +8922,7 @@
         <v>218</v>
       </c>
       <c r="L59" t="s" s="2">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="M59" t="s" s="2">
         <v>220</v>
@@ -9004,7 +9007,7 @@
     </row>
     <row r="60">
       <c r="A60" t="s" s="2">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="B60" t="s" s="2">
         <v>229</v>
@@ -9116,7 +9119,7 @@
     </row>
     <row r="61">
       <c r="A61" t="s" s="2">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="B61" t="s" s="2">
         <v>230</v>
@@ -9230,7 +9233,7 @@
     </row>
     <row r="62">
       <c r="A62" t="s" s="2">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="B62" t="s" s="2">
         <v>231</v>
@@ -9344,7 +9347,7 @@
     </row>
     <row r="63">
       <c r="A63" t="s" s="2">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="B63" t="s" s="2">
         <v>240</v>
@@ -9458,10 +9461,10 @@
     </row>
     <row r="64">
       <c r="A64" t="s" s="2">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="B64" t="s" s="2">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="C64" s="2"/>
       <c r="D64" t="s" s="2">
@@ -9570,10 +9573,10 @@
     </row>
     <row r="65">
       <c r="A65" t="s" s="2">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="B65" t="s" s="2">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="C65" s="2"/>
       <c r="D65" t="s" s="2">
@@ -9684,10 +9687,10 @@
     </row>
     <row r="66">
       <c r="A66" t="s" s="2">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="B66" t="s" s="2">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="C66" s="2"/>
       <c r="D66" t="s" s="2">
@@ -9713,16 +9716,16 @@
         <v>147</v>
       </c>
       <c r="L66" t="s" s="2">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="M66" t="s" s="2">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="N66" t="s" s="2">
-        <v>341</v>
+        <v>342</v>
       </c>
       <c r="O66" t="s" s="2">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="P66" t="s" s="2">
         <v>78</v>
@@ -9771,7 +9774,7 @@
         <v>78</v>
       </c>
       <c r="AF66" t="s" s="2">
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="AG66" t="s" s="2">
         <v>79</v>
@@ -9786,10 +9789,10 @@
         <v>100</v>
       </c>
       <c r="AK66" t="s" s="2">
-        <v>344</v>
+        <v>345</v>
       </c>
       <c r="AL66" t="s" s="2">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="AM66" t="s" s="2">
         <v>78</v>
@@ -9800,10 +9803,10 @@
     </row>
     <row r="67">
       <c r="A67" t="s" s="2">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="B67" t="s" s="2">
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="C67" s="2"/>
       <c r="D67" t="s" s="2">
@@ -9912,10 +9915,10 @@
     </row>
     <row r="68">
       <c r="A68" t="s" s="2">
-        <v>348</v>
+        <v>349</v>
       </c>
       <c r="B68" t="s" s="2">
-        <v>349</v>
+        <v>350</v>
       </c>
       <c r="C68" s="2"/>
       <c r="D68" t="s" s="2">
@@ -10026,10 +10029,10 @@
     </row>
     <row r="69">
       <c r="A69" t="s" s="2">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="B69" t="s" s="2">
-        <v>351</v>
+        <v>352</v>
       </c>
       <c r="C69" s="2"/>
       <c r="D69" t="s" s="2">
@@ -10055,16 +10058,16 @@
         <v>130</v>
       </c>
       <c r="L69" t="s" s="2">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="M69" t="s" s="2">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="N69" t="s" s="2">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="O69" t="s" s="2">
-        <v>355</v>
+        <v>356</v>
       </c>
       <c r="P69" t="s" s="2">
         <v>78</v>
@@ -10074,7 +10077,7 @@
         <v>78</v>
       </c>
       <c r="S69" t="s" s="2">
-        <v>356</v>
+        <v>357</v>
       </c>
       <c r="T69" t="s" s="2">
         <v>78</v>
@@ -10113,7 +10116,7 @@
         <v>78</v>
       </c>
       <c r="AF69" t="s" s="2">
-        <v>357</v>
+        <v>358</v>
       </c>
       <c r="AG69" t="s" s="2">
         <v>79</v>
@@ -10128,10 +10131,10 @@
         <v>100</v>
       </c>
       <c r="AK69" t="s" s="2">
-        <v>358</v>
+        <v>359</v>
       </c>
       <c r="AL69" t="s" s="2">
-        <v>359</v>
+        <v>360</v>
       </c>
       <c r="AM69" t="s" s="2">
         <v>78</v>
@@ -10142,10 +10145,10 @@
     </row>
     <row r="70">
       <c r="A70" t="s" s="2">
-        <v>360</v>
+        <v>361</v>
       </c>
       <c r="B70" t="s" s="2">
-        <v>361</v>
+        <v>362</v>
       </c>
       <c r="C70" s="2"/>
       <c r="D70" t="s" s="2">
@@ -10171,13 +10174,13 @@
         <v>102</v>
       </c>
       <c r="L70" t="s" s="2">
-        <v>362</v>
+        <v>363</v>
       </c>
       <c r="M70" t="s" s="2">
-        <v>363</v>
+        <v>364</v>
       </c>
       <c r="N70" t="s" s="2">
-        <v>364</v>
+        <v>365</v>
       </c>
       <c r="O70" s="2"/>
       <c r="P70" t="s" s="2">
@@ -10227,7 +10230,7 @@
         <v>78</v>
       </c>
       <c r="AF70" t="s" s="2">
-        <v>365</v>
+        <v>366</v>
       </c>
       <c r="AG70" t="s" s="2">
         <v>79</v>
@@ -10242,10 +10245,10 @@
         <v>100</v>
       </c>
       <c r="AK70" t="s" s="2">
-        <v>366</v>
+        <v>367</v>
       </c>
       <c r="AL70" t="s" s="2">
-        <v>367</v>
+        <v>368</v>
       </c>
       <c r="AM70" t="s" s="2">
         <v>78</v>
@@ -10256,10 +10259,10 @@
     </row>
     <row r="71">
       <c r="A71" t="s" s="2">
-        <v>368</v>
+        <v>369</v>
       </c>
       <c r="B71" t="s" s="2">
-        <v>369</v>
+        <v>370</v>
       </c>
       <c r="C71" s="2"/>
       <c r="D71" t="s" s="2">
@@ -10285,14 +10288,14 @@
         <v>169</v>
       </c>
       <c r="L71" t="s" s="2">
-        <v>370</v>
+        <v>371</v>
       </c>
       <c r="M71" t="s" s="2">
-        <v>371</v>
+        <v>372</v>
       </c>
       <c r="N71" s="2"/>
       <c r="O71" t="s" s="2">
-        <v>372</v>
+        <v>373</v>
       </c>
       <c r="P71" t="s" s="2">
         <v>78</v>
@@ -10341,7 +10344,7 @@
         <v>78</v>
       </c>
       <c r="AF71" t="s" s="2">
-        <v>373</v>
+        <v>374</v>
       </c>
       <c r="AG71" t="s" s="2">
         <v>79</v>
@@ -10356,10 +10359,10 @@
         <v>100</v>
       </c>
       <c r="AK71" t="s" s="2">
-        <v>374</v>
+        <v>375</v>
       </c>
       <c r="AL71" t="s" s="2">
-        <v>375</v>
+        <v>376</v>
       </c>
       <c r="AM71" t="s" s="2">
         <v>78</v>
@@ -10370,10 +10373,10 @@
     </row>
     <row r="72">
       <c r="A72" t="s" s="2">
-        <v>376</v>
+        <v>377</v>
       </c>
       <c r="B72" t="s" s="2">
-        <v>377</v>
+        <v>378</v>
       </c>
       <c r="C72" s="2"/>
       <c r="D72" t="s" s="2">
@@ -10399,14 +10402,14 @@
         <v>102</v>
       </c>
       <c r="L72" t="s" s="2">
-        <v>378</v>
+        <v>379</v>
       </c>
       <c r="M72" t="s" s="2">
-        <v>379</v>
+        <v>380</v>
       </c>
       <c r="N72" s="2"/>
       <c r="O72" t="s" s="2">
-        <v>380</v>
+        <v>381</v>
       </c>
       <c r="P72" t="s" s="2">
         <v>78</v>
@@ -10455,7 +10458,7 @@
         <v>78</v>
       </c>
       <c r="AF72" t="s" s="2">
-        <v>381</v>
+        <v>382</v>
       </c>
       <c r="AG72" t="s" s="2">
         <v>79</v>
@@ -10470,10 +10473,10 @@
         <v>100</v>
       </c>
       <c r="AK72" t="s" s="2">
-        <v>382</v>
+        <v>383</v>
       </c>
       <c r="AL72" t="s" s="2">
-        <v>383</v>
+        <v>384</v>
       </c>
       <c r="AM72" t="s" s="2">
         <v>78</v>
@@ -10484,10 +10487,10 @@
     </row>
     <row r="73">
       <c r="A73" t="s" s="2">
-        <v>384</v>
+        <v>385</v>
       </c>
       <c r="B73" t="s" s="2">
-        <v>385</v>
+        <v>386</v>
       </c>
       <c r="C73" s="2"/>
       <c r="D73" t="s" s="2">
@@ -10510,19 +10513,19 @@
         <v>89</v>
       </c>
       <c r="K73" t="s" s="2">
-        <v>386</v>
+        <v>387</v>
       </c>
       <c r="L73" t="s" s="2">
-        <v>387</v>
+        <v>388</v>
       </c>
       <c r="M73" t="s" s="2">
-        <v>388</v>
+        <v>389</v>
       </c>
       <c r="N73" t="s" s="2">
-        <v>389</v>
+        <v>390</v>
       </c>
       <c r="O73" t="s" s="2">
-        <v>390</v>
+        <v>391</v>
       </c>
       <c r="P73" t="s" s="2">
         <v>78</v>
@@ -10571,7 +10574,7 @@
         <v>78</v>
       </c>
       <c r="AF73" t="s" s="2">
-        <v>391</v>
+        <v>392</v>
       </c>
       <c r="AG73" t="s" s="2">
         <v>79</v>
@@ -10586,10 +10589,10 @@
         <v>100</v>
       </c>
       <c r="AK73" t="s" s="2">
-        <v>392</v>
+        <v>393</v>
       </c>
       <c r="AL73" t="s" s="2">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="AM73" t="s" s="2">
         <v>78</v>
@@ -10600,10 +10603,10 @@
     </row>
     <row r="74">
       <c r="A74" t="s" s="2">
-        <v>394</v>
+        <v>395</v>
       </c>
       <c r="B74" t="s" s="2">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="C74" s="2"/>
       <c r="D74" t="s" s="2">
@@ -10629,16 +10632,16 @@
         <v>102</v>
       </c>
       <c r="L74" t="s" s="2">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="M74" t="s" s="2">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="N74" t="s" s="2">
-        <v>398</v>
+        <v>399</v>
       </c>
       <c r="O74" t="s" s="2">
-        <v>399</v>
+        <v>400</v>
       </c>
       <c r="P74" t="s" s="2">
         <v>78</v>
@@ -10687,7 +10690,7 @@
         <v>78</v>
       </c>
       <c r="AF74" t="s" s="2">
-        <v>400</v>
+        <v>401</v>
       </c>
       <c r="AG74" t="s" s="2">
         <v>79</v>
@@ -10702,10 +10705,10 @@
         <v>100</v>
       </c>
       <c r="AK74" t="s" s="2">
-        <v>401</v>
+        <v>402</v>
       </c>
       <c r="AL74" t="s" s="2">
-        <v>402</v>
+        <v>403</v>
       </c>
       <c r="AM74" t="s" s="2">
         <v>78</v>
@@ -10716,7 +10719,7 @@
     </row>
     <row r="75">
       <c r="A75" t="s" s="2">
-        <v>403</v>
+        <v>404</v>
       </c>
       <c r="B75" t="s" s="2">
         <v>249</v>
@@ -10764,7 +10767,7 @@
         <v>78</v>
       </c>
       <c r="S75" t="s" s="2">
-        <v>404</v>
+        <v>405</v>
       </c>
       <c r="T75" t="s" s="2">
         <v>254</v>
@@ -10832,7 +10835,7 @@
     </row>
     <row r="76">
       <c r="A76" t="s" s="2">
-        <v>405</v>
+        <v>406</v>
       </c>
       <c r="B76" t="s" s="2">
         <v>259</v>
@@ -10946,7 +10949,7 @@
     </row>
     <row r="77">
       <c r="A77" t="s" s="2">
-        <v>406</v>
+        <v>407</v>
       </c>
       <c r="B77" t="s" s="2">
         <v>268</v>
@@ -11058,7 +11061,7 @@
     </row>
     <row r="78">
       <c r="A78" t="s" s="2">
-        <v>407</v>
+        <v>408</v>
       </c>
       <c r="B78" t="s" s="2">
         <v>276</v>
@@ -11172,13 +11175,13 @@
     </row>
     <row r="79">
       <c r="A79" t="s" s="2">
-        <v>408</v>
+        <v>409</v>
       </c>
       <c r="B79" t="s" s="2">
         <v>217</v>
       </c>
       <c r="C79" t="s" s="2">
-        <v>409</v>
+        <v>410</v>
       </c>
       <c r="D79" t="s" s="2">
         <v>78</v>
@@ -11203,7 +11206,7 @@
         <v>218</v>
       </c>
       <c r="L79" t="s" s="2">
-        <v>410</v>
+        <v>411</v>
       </c>
       <c r="M79" t="s" s="2">
         <v>220</v>
@@ -11288,7 +11291,7 @@
     </row>
     <row r="80">
       <c r="A80" t="s" s="2">
-        <v>411</v>
+        <v>412</v>
       </c>
       <c r="B80" t="s" s="2">
         <v>229</v>
@@ -11400,7 +11403,7 @@
     </row>
     <row r="81">
       <c r="A81" t="s" s="2">
-        <v>412</v>
+        <v>413</v>
       </c>
       <c r="B81" t="s" s="2">
         <v>230</v>
@@ -11514,7 +11517,7 @@
     </row>
     <row r="82">
       <c r="A82" t="s" s="2">
-        <v>413</v>
+        <v>414</v>
       </c>
       <c r="B82" t="s" s="2">
         <v>231</v>
@@ -11628,7 +11631,7 @@
     </row>
     <row r="83">
       <c r="A83" t="s" s="2">
-        <v>414</v>
+        <v>415</v>
       </c>
       <c r="B83" t="s" s="2">
         <v>240</v>
@@ -11676,7 +11679,7 @@
         <v>78</v>
       </c>
       <c r="S83" t="s" s="2">
-        <v>415</v>
+        <v>416</v>
       </c>
       <c r="T83" t="s" s="2">
         <v>78</v>
@@ -11742,7 +11745,7 @@
     </row>
     <row r="84">
       <c r="A84" t="s" s="2">
-        <v>416</v>
+        <v>417</v>
       </c>
       <c r="B84" t="s" s="2">
         <v>249</v>
@@ -11790,7 +11793,7 @@
         <v>78</v>
       </c>
       <c r="S84" t="s" s="2">
-        <v>417</v>
+        <v>418</v>
       </c>
       <c r="T84" t="s" s="2">
         <v>254</v>
@@ -11858,7 +11861,7 @@
     </row>
     <row r="85">
       <c r="A85" t="s" s="2">
-        <v>418</v>
+        <v>419</v>
       </c>
       <c r="B85" t="s" s="2">
         <v>259</v>
@@ -11972,7 +11975,7 @@
     </row>
     <row r="86">
       <c r="A86" t="s" s="2">
-        <v>419</v>
+        <v>420</v>
       </c>
       <c r="B86" t="s" s="2">
         <v>268</v>
@@ -12084,7 +12087,7 @@
     </row>
     <row r="87">
       <c r="A87" t="s" s="2">
-        <v>420</v>
+        <v>421</v>
       </c>
       <c r="B87" t="s" s="2">
         <v>276</v>
@@ -12198,10 +12201,10 @@
     </row>
     <row r="88">
       <c r="A88" t="s" s="2">
-        <v>421</v>
+        <v>422</v>
       </c>
       <c r="B88" t="s" s="2">
-        <v>421</v>
+        <v>422</v>
       </c>
       <c r="C88" s="2"/>
       <c r="D88" t="s" s="2">
@@ -12224,70 +12227,70 @@
         <v>89</v>
       </c>
       <c r="K88" t="s" s="2">
-        <v>386</v>
+        <v>387</v>
       </c>
       <c r="L88" t="s" s="2">
+        <v>423</v>
+      </c>
+      <c r="M88" t="s" s="2">
+        <v>424</v>
+      </c>
+      <c r="N88" t="s" s="2">
+        <v>425</v>
+      </c>
+      <c r="O88" t="s" s="2">
+        <v>426</v>
+      </c>
+      <c r="P88" t="s" s="2">
+        <v>78</v>
+      </c>
+      <c r="Q88" t="s" s="2">
+        <v>427</v>
+      </c>
+      <c r="R88" t="s" s="2">
+        <v>78</v>
+      </c>
+      <c r="S88" t="s" s="2">
+        <v>78</v>
+      </c>
+      <c r="T88" t="s" s="2">
+        <v>78</v>
+      </c>
+      <c r="U88" t="s" s="2">
+        <v>78</v>
+      </c>
+      <c r="V88" t="s" s="2">
+        <v>78</v>
+      </c>
+      <c r="W88" t="s" s="2">
+        <v>78</v>
+      </c>
+      <c r="X88" t="s" s="2">
+        <v>78</v>
+      </c>
+      <c r="Y88" t="s" s="2">
+        <v>78</v>
+      </c>
+      <c r="Z88" t="s" s="2">
+        <v>78</v>
+      </c>
+      <c r="AA88" t="s" s="2">
+        <v>78</v>
+      </c>
+      <c r="AB88" t="s" s="2">
+        <v>78</v>
+      </c>
+      <c r="AC88" t="s" s="2">
+        <v>78</v>
+      </c>
+      <c r="AD88" t="s" s="2">
+        <v>78</v>
+      </c>
+      <c r="AE88" t="s" s="2">
+        <v>78</v>
+      </c>
+      <c r="AF88" t="s" s="2">
         <v>422</v>
-      </c>
-      <c r="M88" t="s" s="2">
-        <v>423</v>
-      </c>
-      <c r="N88" t="s" s="2">
-        <v>424</v>
-      </c>
-      <c r="O88" t="s" s="2">
-        <v>425</v>
-      </c>
-      <c r="P88" t="s" s="2">
-        <v>78</v>
-      </c>
-      <c r="Q88" t="s" s="2">
-        <v>426</v>
-      </c>
-      <c r="R88" t="s" s="2">
-        <v>78</v>
-      </c>
-      <c r="S88" t="s" s="2">
-        <v>78</v>
-      </c>
-      <c r="T88" t="s" s="2">
-        <v>78</v>
-      </c>
-      <c r="U88" t="s" s="2">
-        <v>78</v>
-      </c>
-      <c r="V88" t="s" s="2">
-        <v>78</v>
-      </c>
-      <c r="W88" t="s" s="2">
-        <v>78</v>
-      </c>
-      <c r="X88" t="s" s="2">
-        <v>78</v>
-      </c>
-      <c r="Y88" t="s" s="2">
-        <v>78</v>
-      </c>
-      <c r="Z88" t="s" s="2">
-        <v>78</v>
-      </c>
-      <c r="AA88" t="s" s="2">
-        <v>78</v>
-      </c>
-      <c r="AB88" t="s" s="2">
-        <v>78</v>
-      </c>
-      <c r="AC88" t="s" s="2">
-        <v>78</v>
-      </c>
-      <c r="AD88" t="s" s="2">
-        <v>78</v>
-      </c>
-      <c r="AE88" t="s" s="2">
-        <v>78</v>
-      </c>
-      <c r="AF88" t="s" s="2">
-        <v>421</v>
       </c>
       <c r="AG88" t="s" s="2">
         <v>79</v>
@@ -12302,24 +12305,24 @@
         <v>100</v>
       </c>
       <c r="AK88" t="s" s="2">
-        <v>427</v>
+        <v>428</v>
       </c>
       <c r="AL88" t="s" s="2">
-        <v>428</v>
+        <v>429</v>
       </c>
       <c r="AM88" t="s" s="2">
-        <v>429</v>
+        <v>430</v>
       </c>
       <c r="AN88" t="s" s="2">
-        <v>430</v>
+        <v>431</v>
       </c>
     </row>
     <row r="89">
       <c r="A89" t="s" s="2">
-        <v>431</v>
+        <v>432</v>
       </c>
       <c r="B89" t="s" s="2">
-        <v>431</v>
+        <v>432</v>
       </c>
       <c r="C89" s="2"/>
       <c r="D89" t="s" s="2">
@@ -12345,16 +12348,16 @@
         <v>241</v>
       </c>
       <c r="L89" t="s" s="2">
-        <v>432</v>
+        <v>433</v>
       </c>
       <c r="M89" t="s" s="2">
-        <v>433</v>
+        <v>434</v>
       </c>
       <c r="N89" t="s" s="2">
-        <v>434</v>
+        <v>435</v>
       </c>
       <c r="O89" t="s" s="2">
-        <v>435</v>
+        <v>436</v>
       </c>
       <c r="P89" t="s" s="2">
         <v>78</v>
@@ -12382,10 +12385,10 @@
         <v>159</v>
       </c>
       <c r="Y89" t="s" s="2">
-        <v>436</v>
+        <v>437</v>
       </c>
       <c r="Z89" t="s" s="2">
-        <v>437</v>
+        <v>438</v>
       </c>
       <c r="AA89" t="s" s="2">
         <v>78</v>
@@ -12401,7 +12404,7 @@
         <v>115</v>
       </c>
       <c r="AF89" t="s" s="2">
-        <v>431</v>
+        <v>432</v>
       </c>
       <c r="AG89" t="s" s="2">
         <v>79</v>
@@ -12416,27 +12419,27 @@
         <v>100</v>
       </c>
       <c r="AK89" t="s" s="2">
-        <v>438</v>
+        <v>439</v>
       </c>
       <c r="AL89" t="s" s="2">
-        <v>439</v>
+        <v>440</v>
       </c>
       <c r="AM89" t="s" s="2">
         <v>106</v>
       </c>
       <c r="AN89" t="s" s="2">
-        <v>440</v>
+        <v>441</v>
       </c>
     </row>
     <row r="90">
       <c r="A90" t="s" s="2">
-        <v>441</v>
+        <v>442</v>
       </c>
       <c r="B90" t="s" s="2">
-        <v>431</v>
+        <v>432</v>
       </c>
       <c r="C90" t="s" s="2">
-        <v>442</v>
+        <v>443</v>
       </c>
       <c r="D90" t="s" s="2">
         <v>78</v>
@@ -12461,16 +12464,16 @@
         <v>241</v>
       </c>
       <c r="L90" t="s" s="2">
-        <v>432</v>
+        <v>433</v>
       </c>
       <c r="M90" t="s" s="2">
-        <v>433</v>
+        <v>434</v>
       </c>
       <c r="N90" t="s" s="2">
-        <v>434</v>
+        <v>435</v>
       </c>
       <c r="O90" t="s" s="2">
-        <v>435</v>
+        <v>436</v>
       </c>
       <c r="P90" t="s" s="2">
         <v>78</v>
@@ -12499,7 +12502,7 @@
       </c>
       <c r="Y90" s="2"/>
       <c r="Z90" t="s" s="2">
-        <v>443</v>
+        <v>444</v>
       </c>
       <c r="AA90" t="s" s="2">
         <v>78</v>
@@ -12517,7 +12520,7 @@
         <v>78</v>
       </c>
       <c r="AF90" t="s" s="2">
-        <v>431</v>
+        <v>432</v>
       </c>
       <c r="AG90" t="s" s="2">
         <v>79</v>
@@ -12532,24 +12535,24 @@
         <v>100</v>
       </c>
       <c r="AK90" t="s" s="2">
-        <v>438</v>
+        <v>439</v>
       </c>
       <c r="AL90" t="s" s="2">
-        <v>439</v>
+        <v>440</v>
       </c>
       <c r="AM90" t="s" s="2">
         <v>106</v>
       </c>
       <c r="AN90" t="s" s="2">
-        <v>440</v>
+        <v>441</v>
       </c>
     </row>
     <row r="91">
       <c r="A91" t="s" s="2">
-        <v>444</v>
+        <v>445</v>
       </c>
       <c r="B91" t="s" s="2">
-        <v>445</v>
+        <v>446</v>
       </c>
       <c r="C91" s="2"/>
       <c r="D91" t="s" s="2">
@@ -12658,10 +12661,10 @@
     </row>
     <row r="92">
       <c r="A92" t="s" s="2">
-        <v>446</v>
+        <v>447</v>
       </c>
       <c r="B92" t="s" s="2">
-        <v>447</v>
+        <v>448</v>
       </c>
       <c r="C92" s="2"/>
       <c r="D92" t="s" s="2">
@@ -12772,10 +12775,10 @@
     </row>
     <row r="93">
       <c r="A93" t="s" s="2">
-        <v>448</v>
+        <v>449</v>
       </c>
       <c r="B93" t="s" s="2">
-        <v>449</v>
+        <v>450</v>
       </c>
       <c r="C93" s="2"/>
       <c r="D93" t="s" s="2">
@@ -12801,16 +12804,16 @@
         <v>147</v>
       </c>
       <c r="L93" t="s" s="2">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="M93" t="s" s="2">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="N93" t="s" s="2">
-        <v>341</v>
+        <v>342</v>
       </c>
       <c r="O93" t="s" s="2">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="P93" t="s" s="2">
         <v>78</v>
@@ -12859,7 +12862,7 @@
         <v>78</v>
       </c>
       <c r="AF93" t="s" s="2">
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="AG93" t="s" s="2">
         <v>79</v>
@@ -12874,10 +12877,10 @@
         <v>100</v>
       </c>
       <c r="AK93" t="s" s="2">
-        <v>344</v>
+        <v>345</v>
       </c>
       <c r="AL93" t="s" s="2">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="AM93" t="s" s="2">
         <v>78</v>
@@ -12888,10 +12891,10 @@
     </row>
     <row r="94">
       <c r="A94" t="s" s="2">
-        <v>450</v>
+        <v>451</v>
       </c>
       <c r="B94" t="s" s="2">
-        <v>451</v>
+        <v>452</v>
       </c>
       <c r="C94" s="2"/>
       <c r="D94" t="s" s="2">
@@ -13000,10 +13003,10 @@
     </row>
     <row r="95">
       <c r="A95" t="s" s="2">
-        <v>452</v>
+        <v>453</v>
       </c>
       <c r="B95" t="s" s="2">
-        <v>453</v>
+        <v>454</v>
       </c>
       <c r="C95" s="2"/>
       <c r="D95" t="s" s="2">
@@ -13114,10 +13117,10 @@
     </row>
     <row r="96">
       <c r="A96" t="s" s="2">
-        <v>454</v>
+        <v>455</v>
       </c>
       <c r="B96" t="s" s="2">
-        <v>455</v>
+        <v>456</v>
       </c>
       <c r="C96" s="2"/>
       <c r="D96" t="s" s="2">
@@ -13143,16 +13146,16 @@
         <v>130</v>
       </c>
       <c r="L96" t="s" s="2">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="M96" t="s" s="2">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="N96" t="s" s="2">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="O96" t="s" s="2">
-        <v>355</v>
+        <v>356</v>
       </c>
       <c r="P96" t="s" s="2">
         <v>78</v>
@@ -13201,7 +13204,7 @@
         <v>78</v>
       </c>
       <c r="AF96" t="s" s="2">
-        <v>357</v>
+        <v>358</v>
       </c>
       <c r="AG96" t="s" s="2">
         <v>79</v>
@@ -13216,10 +13219,10 @@
         <v>100</v>
       </c>
       <c r="AK96" t="s" s="2">
-        <v>358</v>
+        <v>359</v>
       </c>
       <c r="AL96" t="s" s="2">
-        <v>359</v>
+        <v>360</v>
       </c>
       <c r="AM96" t="s" s="2">
         <v>78</v>
@@ -13230,10 +13233,10 @@
     </row>
     <row r="97">
       <c r="A97" t="s" s="2">
-        <v>456</v>
+        <v>457</v>
       </c>
       <c r="B97" t="s" s="2">
-        <v>457</v>
+        <v>458</v>
       </c>
       <c r="C97" s="2"/>
       <c r="D97" t="s" s="2">
@@ -13259,13 +13262,13 @@
         <v>102</v>
       </c>
       <c r="L97" t="s" s="2">
-        <v>362</v>
+        <v>363</v>
       </c>
       <c r="M97" t="s" s="2">
-        <v>363</v>
+        <v>364</v>
       </c>
       <c r="N97" t="s" s="2">
-        <v>364</v>
+        <v>365</v>
       </c>
       <c r="O97" s="2"/>
       <c r="P97" t="s" s="2">
@@ -13315,7 +13318,7 @@
         <v>78</v>
       </c>
       <c r="AF97" t="s" s="2">
-        <v>365</v>
+        <v>366</v>
       </c>
       <c r="AG97" t="s" s="2">
         <v>79</v>
@@ -13330,10 +13333,10 @@
         <v>100</v>
       </c>
       <c r="AK97" t="s" s="2">
-        <v>366</v>
+        <v>367</v>
       </c>
       <c r="AL97" t="s" s="2">
-        <v>367</v>
+        <v>368</v>
       </c>
       <c r="AM97" t="s" s="2">
         <v>78</v>
@@ -13344,10 +13347,10 @@
     </row>
     <row r="98">
       <c r="A98" t="s" s="2">
-        <v>458</v>
+        <v>459</v>
       </c>
       <c r="B98" t="s" s="2">
-        <v>459</v>
+        <v>460</v>
       </c>
       <c r="C98" s="2"/>
       <c r="D98" t="s" s="2">
@@ -13373,14 +13376,14 @@
         <v>169</v>
       </c>
       <c r="L98" t="s" s="2">
-        <v>460</v>
+        <v>461</v>
       </c>
       <c r="M98" t="s" s="2">
-        <v>371</v>
+        <v>372</v>
       </c>
       <c r="N98" s="2"/>
       <c r="O98" t="s" s="2">
-        <v>372</v>
+        <v>373</v>
       </c>
       <c r="P98" t="s" s="2">
         <v>78</v>
@@ -13429,7 +13432,7 @@
         <v>78</v>
       </c>
       <c r="AF98" t="s" s="2">
-        <v>373</v>
+        <v>374</v>
       </c>
       <c r="AG98" t="s" s="2">
         <v>79</v>
@@ -13444,10 +13447,10 @@
         <v>100</v>
       </c>
       <c r="AK98" t="s" s="2">
-        <v>374</v>
+        <v>375</v>
       </c>
       <c r="AL98" t="s" s="2">
-        <v>375</v>
+        <v>376</v>
       </c>
       <c r="AM98" t="s" s="2">
         <v>78</v>
@@ -13458,10 +13461,10 @@
     </row>
     <row r="99">
       <c r="A99" t="s" s="2">
-        <v>461</v>
+        <v>462</v>
       </c>
       <c r="B99" t="s" s="2">
-        <v>462</v>
+        <v>463</v>
       </c>
       <c r="C99" s="2"/>
       <c r="D99" t="s" s="2">
@@ -13487,14 +13490,14 @@
         <v>102</v>
       </c>
       <c r="L99" t="s" s="2">
-        <v>378</v>
+        <v>379</v>
       </c>
       <c r="M99" t="s" s="2">
-        <v>379</v>
+        <v>380</v>
       </c>
       <c r="N99" s="2"/>
       <c r="O99" t="s" s="2">
-        <v>380</v>
+        <v>381</v>
       </c>
       <c r="P99" t="s" s="2">
         <v>78</v>
@@ -13543,7 +13546,7 @@
         <v>78</v>
       </c>
       <c r="AF99" t="s" s="2">
-        <v>381</v>
+        <v>382</v>
       </c>
       <c r="AG99" t="s" s="2">
         <v>79</v>
@@ -13558,10 +13561,10 @@
         <v>100</v>
       </c>
       <c r="AK99" t="s" s="2">
-        <v>382</v>
+        <v>383</v>
       </c>
       <c r="AL99" t="s" s="2">
-        <v>383</v>
+        <v>384</v>
       </c>
       <c r="AM99" t="s" s="2">
         <v>78</v>
@@ -13572,10 +13575,10 @@
     </row>
     <row r="100">
       <c r="A100" t="s" s="2">
-        <v>463</v>
+        <v>464</v>
       </c>
       <c r="B100" t="s" s="2">
-        <v>464</v>
+        <v>465</v>
       </c>
       <c r="C100" s="2"/>
       <c r="D100" t="s" s="2">
@@ -13598,19 +13601,19 @@
         <v>89</v>
       </c>
       <c r="K100" t="s" s="2">
-        <v>386</v>
+        <v>387</v>
       </c>
       <c r="L100" t="s" s="2">
-        <v>387</v>
+        <v>388</v>
       </c>
       <c r="M100" t="s" s="2">
-        <v>388</v>
+        <v>389</v>
       </c>
       <c r="N100" t="s" s="2">
-        <v>389</v>
+        <v>390</v>
       </c>
       <c r="O100" t="s" s="2">
-        <v>390</v>
+        <v>391</v>
       </c>
       <c r="P100" t="s" s="2">
         <v>78</v>
@@ -13659,7 +13662,7 @@
         <v>78</v>
       </c>
       <c r="AF100" t="s" s="2">
-        <v>391</v>
+        <v>392</v>
       </c>
       <c r="AG100" t="s" s="2">
         <v>79</v>
@@ -13674,10 +13677,10 @@
         <v>100</v>
       </c>
       <c r="AK100" t="s" s="2">
-        <v>392</v>
+        <v>393</v>
       </c>
       <c r="AL100" t="s" s="2">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="AM100" t="s" s="2">
         <v>78</v>
@@ -13688,10 +13691,10 @@
     </row>
     <row r="101">
       <c r="A101" t="s" s="2">
-        <v>465</v>
+        <v>466</v>
       </c>
       <c r="B101" t="s" s="2">
-        <v>466</v>
+        <v>467</v>
       </c>
       <c r="C101" s="2"/>
       <c r="D101" t="s" s="2">
@@ -13717,16 +13720,16 @@
         <v>102</v>
       </c>
       <c r="L101" t="s" s="2">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="M101" t="s" s="2">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="N101" t="s" s="2">
-        <v>398</v>
+        <v>399</v>
       </c>
       <c r="O101" t="s" s="2">
-        <v>399</v>
+        <v>400</v>
       </c>
       <c r="P101" t="s" s="2">
         <v>78</v>
@@ -13775,7 +13778,7 @@
         <v>78</v>
       </c>
       <c r="AF101" t="s" s="2">
-        <v>400</v>
+        <v>401</v>
       </c>
       <c r="AG101" t="s" s="2">
         <v>79</v>
@@ -13790,10 +13793,10 @@
         <v>100</v>
       </c>
       <c r="AK101" t="s" s="2">
-        <v>401</v>
+        <v>402</v>
       </c>
       <c r="AL101" t="s" s="2">
-        <v>402</v>
+        <v>403</v>
       </c>
       <c r="AM101" t="s" s="2">
         <v>78</v>
@@ -13804,13 +13807,13 @@
     </row>
     <row r="102">
       <c r="A102" t="s" s="2">
-        <v>467</v>
+        <v>468</v>
       </c>
       <c r="B102" t="s" s="2">
-        <v>431</v>
+        <v>432</v>
       </c>
       <c r="C102" t="s" s="2">
-        <v>468</v>
+        <v>469</v>
       </c>
       <c r="D102" t="s" s="2">
         <v>78</v>
@@ -13835,16 +13838,16 @@
         <v>241</v>
       </c>
       <c r="L102" t="s" s="2">
-        <v>469</v>
+        <v>470</v>
       </c>
       <c r="M102" t="s" s="2">
-        <v>433</v>
+        <v>434</v>
       </c>
       <c r="N102" t="s" s="2">
-        <v>434</v>
+        <v>435</v>
       </c>
       <c r="O102" t="s" s="2">
-        <v>435</v>
+        <v>436</v>
       </c>
       <c r="P102" t="s" s="2">
         <v>78</v>
@@ -13873,7 +13876,7 @@
       </c>
       <c r="Y102" s="2"/>
       <c r="Z102" t="s" s="2">
-        <v>470</v>
+        <v>471</v>
       </c>
       <c r="AA102" t="s" s="2">
         <v>78</v>
@@ -13891,7 +13894,7 @@
         <v>78</v>
       </c>
       <c r="AF102" t="s" s="2">
-        <v>431</v>
+        <v>432</v>
       </c>
       <c r="AG102" t="s" s="2">
         <v>79</v>
@@ -13906,24 +13909,24 @@
         <v>100</v>
       </c>
       <c r="AK102" t="s" s="2">
-        <v>438</v>
+        <v>439</v>
       </c>
       <c r="AL102" t="s" s="2">
-        <v>439</v>
+        <v>440</v>
       </c>
       <c r="AM102" t="s" s="2">
         <v>106</v>
       </c>
       <c r="AN102" t="s" s="2">
-        <v>440</v>
+        <v>441</v>
       </c>
     </row>
     <row r="103">
       <c r="A103" t="s" s="2">
-        <v>471</v>
+        <v>472</v>
       </c>
       <c r="B103" t="s" s="2">
-        <v>445</v>
+        <v>446</v>
       </c>
       <c r="C103" s="2"/>
       <c r="D103" t="s" s="2">
@@ -14032,10 +14035,10 @@
     </row>
     <row r="104">
       <c r="A104" t="s" s="2">
-        <v>472</v>
+        <v>473</v>
       </c>
       <c r="B104" t="s" s="2">
-        <v>447</v>
+        <v>448</v>
       </c>
       <c r="C104" s="2"/>
       <c r="D104" t="s" s="2">
@@ -14146,10 +14149,10 @@
     </row>
     <row r="105">
       <c r="A105" t="s" s="2">
-        <v>473</v>
+        <v>474</v>
       </c>
       <c r="B105" t="s" s="2">
-        <v>449</v>
+        <v>450</v>
       </c>
       <c r="C105" s="2"/>
       <c r="D105" t="s" s="2">
@@ -14175,16 +14178,16 @@
         <v>147</v>
       </c>
       <c r="L105" t="s" s="2">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="M105" t="s" s="2">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="N105" t="s" s="2">
-        <v>341</v>
+        <v>342</v>
       </c>
       <c r="O105" t="s" s="2">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="P105" t="s" s="2">
         <v>78</v>
@@ -14233,7 +14236,7 @@
         <v>78</v>
       </c>
       <c r="AF105" t="s" s="2">
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="AG105" t="s" s="2">
         <v>79</v>
@@ -14248,10 +14251,10 @@
         <v>100</v>
       </c>
       <c r="AK105" t="s" s="2">
-        <v>344</v>
+        <v>345</v>
       </c>
       <c r="AL105" t="s" s="2">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="AM105" t="s" s="2">
         <v>78</v>
@@ -14262,10 +14265,10 @@
     </row>
     <row r="106">
       <c r="A106" t="s" s="2">
-        <v>474</v>
+        <v>475</v>
       </c>
       <c r="B106" t="s" s="2">
-        <v>451</v>
+        <v>452</v>
       </c>
       <c r="C106" s="2"/>
       <c r="D106" t="s" s="2">
@@ -14374,10 +14377,10 @@
     </row>
     <row r="107">
       <c r="A107" t="s" s="2">
-        <v>475</v>
+        <v>476</v>
       </c>
       <c r="B107" t="s" s="2">
-        <v>453</v>
+        <v>454</v>
       </c>
       <c r="C107" s="2"/>
       <c r="D107" t="s" s="2">
@@ -14488,10 +14491,10 @@
     </row>
     <row r="108">
       <c r="A108" t="s" s="2">
-        <v>476</v>
+        <v>477</v>
       </c>
       <c r="B108" t="s" s="2">
-        <v>455</v>
+        <v>456</v>
       </c>
       <c r="C108" s="2"/>
       <c r="D108" t="s" s="2">
@@ -14517,16 +14520,16 @@
         <v>130</v>
       </c>
       <c r="L108" t="s" s="2">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="M108" t="s" s="2">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="N108" t="s" s="2">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="O108" t="s" s="2">
-        <v>355</v>
+        <v>356</v>
       </c>
       <c r="P108" t="s" s="2">
         <v>78</v>
@@ -14575,7 +14578,7 @@
         <v>78</v>
       </c>
       <c r="AF108" t="s" s="2">
-        <v>357</v>
+        <v>358</v>
       </c>
       <c r="AG108" t="s" s="2">
         <v>79</v>
@@ -14590,10 +14593,10 @@
         <v>100</v>
       </c>
       <c r="AK108" t="s" s="2">
-        <v>358</v>
+        <v>359</v>
       </c>
       <c r="AL108" t="s" s="2">
-        <v>359</v>
+        <v>360</v>
       </c>
       <c r="AM108" t="s" s="2">
         <v>78</v>
@@ -14604,10 +14607,10 @@
     </row>
     <row r="109">
       <c r="A109" t="s" s="2">
-        <v>477</v>
+        <v>478</v>
       </c>
       <c r="B109" t="s" s="2">
-        <v>457</v>
+        <v>458</v>
       </c>
       <c r="C109" s="2"/>
       <c r="D109" t="s" s="2">
@@ -14633,13 +14636,13 @@
         <v>102</v>
       </c>
       <c r="L109" t="s" s="2">
-        <v>362</v>
+        <v>363</v>
       </c>
       <c r="M109" t="s" s="2">
-        <v>363</v>
+        <v>364</v>
       </c>
       <c r="N109" t="s" s="2">
-        <v>364</v>
+        <v>365</v>
       </c>
       <c r="O109" s="2"/>
       <c r="P109" t="s" s="2">
@@ -14689,7 +14692,7 @@
         <v>78</v>
       </c>
       <c r="AF109" t="s" s="2">
-        <v>365</v>
+        <v>366</v>
       </c>
       <c r="AG109" t="s" s="2">
         <v>79</v>
@@ -14704,10 +14707,10 @@
         <v>100</v>
       </c>
       <c r="AK109" t="s" s="2">
-        <v>366</v>
+        <v>367</v>
       </c>
       <c r="AL109" t="s" s="2">
-        <v>367</v>
+        <v>368</v>
       </c>
       <c r="AM109" t="s" s="2">
         <v>78</v>
@@ -14718,10 +14721,10 @@
     </row>
     <row r="110">
       <c r="A110" t="s" s="2">
-        <v>478</v>
+        <v>479</v>
       </c>
       <c r="B110" t="s" s="2">
-        <v>459</v>
+        <v>460</v>
       </c>
       <c r="C110" s="2"/>
       <c r="D110" t="s" s="2">
@@ -14747,14 +14750,14 @@
         <v>169</v>
       </c>
       <c r="L110" t="s" s="2">
-        <v>460</v>
+        <v>461</v>
       </c>
       <c r="M110" t="s" s="2">
-        <v>371</v>
+        <v>372</v>
       </c>
       <c r="N110" s="2"/>
       <c r="O110" t="s" s="2">
-        <v>372</v>
+        <v>373</v>
       </c>
       <c r="P110" t="s" s="2">
         <v>78</v>
@@ -14803,7 +14806,7 @@
         <v>78</v>
       </c>
       <c r="AF110" t="s" s="2">
-        <v>373</v>
+        <v>374</v>
       </c>
       <c r="AG110" t="s" s="2">
         <v>79</v>
@@ -14818,10 +14821,10 @@
         <v>100</v>
       </c>
       <c r="AK110" t="s" s="2">
-        <v>374</v>
+        <v>375</v>
       </c>
       <c r="AL110" t="s" s="2">
-        <v>375</v>
+        <v>376</v>
       </c>
       <c r="AM110" t="s" s="2">
         <v>78</v>
@@ -14832,10 +14835,10 @@
     </row>
     <row r="111">
       <c r="A111" t="s" s="2">
-        <v>479</v>
+        <v>480</v>
       </c>
       <c r="B111" t="s" s="2">
-        <v>462</v>
+        <v>463</v>
       </c>
       <c r="C111" s="2"/>
       <c r="D111" t="s" s="2">
@@ -14861,14 +14864,14 @@
         <v>102</v>
       </c>
       <c r="L111" t="s" s="2">
-        <v>378</v>
+        <v>379</v>
       </c>
       <c r="M111" t="s" s="2">
-        <v>379</v>
+        <v>380</v>
       </c>
       <c r="N111" s="2"/>
       <c r="O111" t="s" s="2">
-        <v>380</v>
+        <v>381</v>
       </c>
       <c r="P111" t="s" s="2">
         <v>78</v>
@@ -14917,7 +14920,7 @@
         <v>78</v>
       </c>
       <c r="AF111" t="s" s="2">
-        <v>381</v>
+        <v>382</v>
       </c>
       <c r="AG111" t="s" s="2">
         <v>79</v>
@@ -14932,10 +14935,10 @@
         <v>100</v>
       </c>
       <c r="AK111" t="s" s="2">
-        <v>382</v>
+        <v>383</v>
       </c>
       <c r="AL111" t="s" s="2">
-        <v>383</v>
+        <v>384</v>
       </c>
       <c r="AM111" t="s" s="2">
         <v>78</v>
@@ -14946,10 +14949,10 @@
     </row>
     <row r="112">
       <c r="A112" t="s" s="2">
-        <v>480</v>
+        <v>481</v>
       </c>
       <c r="B112" t="s" s="2">
-        <v>464</v>
+        <v>465</v>
       </c>
       <c r="C112" s="2"/>
       <c r="D112" t="s" s="2">
@@ -14972,19 +14975,19 @@
         <v>89</v>
       </c>
       <c r="K112" t="s" s="2">
-        <v>386</v>
+        <v>387</v>
       </c>
       <c r="L112" t="s" s="2">
-        <v>387</v>
+        <v>388</v>
       </c>
       <c r="M112" t="s" s="2">
-        <v>388</v>
+        <v>389</v>
       </c>
       <c r="N112" t="s" s="2">
-        <v>389</v>
+        <v>390</v>
       </c>
       <c r="O112" t="s" s="2">
-        <v>390</v>
+        <v>391</v>
       </c>
       <c r="P112" t="s" s="2">
         <v>78</v>
@@ -15033,7 +15036,7 @@
         <v>78</v>
       </c>
       <c r="AF112" t="s" s="2">
-        <v>391</v>
+        <v>392</v>
       </c>
       <c r="AG112" t="s" s="2">
         <v>79</v>
@@ -15048,10 +15051,10 @@
         <v>100</v>
       </c>
       <c r="AK112" t="s" s="2">
-        <v>392</v>
+        <v>393</v>
       </c>
       <c r="AL112" t="s" s="2">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="AM112" t="s" s="2">
         <v>78</v>
@@ -15062,10 +15065,10 @@
     </row>
     <row r="113">
       <c r="A113" t="s" s="2">
-        <v>481</v>
+        <v>482</v>
       </c>
       <c r="B113" t="s" s="2">
-        <v>466</v>
+        <v>467</v>
       </c>
       <c r="C113" s="2"/>
       <c r="D113" t="s" s="2">
@@ -15091,16 +15094,16 @@
         <v>102</v>
       </c>
       <c r="L113" t="s" s="2">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="M113" t="s" s="2">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="N113" t="s" s="2">
-        <v>398</v>
+        <v>399</v>
       </c>
       <c r="O113" t="s" s="2">
-        <v>399</v>
+        <v>400</v>
       </c>
       <c r="P113" t="s" s="2">
         <v>78</v>
@@ -15149,7 +15152,7 @@
         <v>78</v>
       </c>
       <c r="AF113" t="s" s="2">
-        <v>400</v>
+        <v>401</v>
       </c>
       <c r="AG113" t="s" s="2">
         <v>79</v>
@@ -15164,10 +15167,10 @@
         <v>100</v>
       </c>
       <c r="AK113" t="s" s="2">
-        <v>401</v>
+        <v>402</v>
       </c>
       <c r="AL113" t="s" s="2">
-        <v>402</v>
+        <v>403</v>
       </c>
       <c r="AM113" t="s" s="2">
         <v>78</v>
@@ -15178,13 +15181,13 @@
     </row>
     <row r="114">
       <c r="A114" t="s" s="2">
-        <v>482</v>
+        <v>483</v>
       </c>
       <c r="B114" t="s" s="2">
-        <v>431</v>
+        <v>432</v>
       </c>
       <c r="C114" t="s" s="2">
-        <v>483</v>
+        <v>484</v>
       </c>
       <c r="D114" t="s" s="2">
         <v>78</v>
@@ -15209,16 +15212,16 @@
         <v>241</v>
       </c>
       <c r="L114" t="s" s="2">
-        <v>484</v>
+        <v>485</v>
       </c>
       <c r="M114" t="s" s="2">
-        <v>433</v>
+        <v>434</v>
       </c>
       <c r="N114" t="s" s="2">
-        <v>434</v>
+        <v>435</v>
       </c>
       <c r="O114" t="s" s="2">
-        <v>435</v>
+        <v>436</v>
       </c>
       <c r="P114" t="s" s="2">
         <v>78</v>
@@ -15247,7 +15250,7 @@
       </c>
       <c r="Y114" s="2"/>
       <c r="Z114" t="s" s="2">
-        <v>485</v>
+        <v>486</v>
       </c>
       <c r="AA114" t="s" s="2">
         <v>78</v>
@@ -15265,7 +15268,7 @@
         <v>78</v>
       </c>
       <c r="AF114" t="s" s="2">
-        <v>431</v>
+        <v>432</v>
       </c>
       <c r="AG114" t="s" s="2">
         <v>79</v>
@@ -15280,24 +15283,24 @@
         <v>100</v>
       </c>
       <c r="AK114" t="s" s="2">
-        <v>438</v>
+        <v>439</v>
       </c>
       <c r="AL114" t="s" s="2">
-        <v>439</v>
+        <v>440</v>
       </c>
       <c r="AM114" t="s" s="2">
         <v>106</v>
       </c>
       <c r="AN114" t="s" s="2">
-        <v>440</v>
+        <v>441</v>
       </c>
     </row>
     <row r="115">
       <c r="A115" t="s" s="2">
-        <v>486</v>
+        <v>487</v>
       </c>
       <c r="B115" t="s" s="2">
-        <v>445</v>
+        <v>446</v>
       </c>
       <c r="C115" s="2"/>
       <c r="D115" t="s" s="2">
@@ -15406,10 +15409,10 @@
     </row>
     <row r="116">
       <c r="A116" t="s" s="2">
-        <v>487</v>
+        <v>488</v>
       </c>
       <c r="B116" t="s" s="2">
-        <v>447</v>
+        <v>448</v>
       </c>
       <c r="C116" s="2"/>
       <c r="D116" t="s" s="2">
@@ -15520,10 +15523,10 @@
     </row>
     <row r="117">
       <c r="A117" t="s" s="2">
-        <v>488</v>
+        <v>489</v>
       </c>
       <c r="B117" t="s" s="2">
-        <v>449</v>
+        <v>450</v>
       </c>
       <c r="C117" s="2"/>
       <c r="D117" t="s" s="2">
@@ -15549,16 +15552,16 @@
         <v>147</v>
       </c>
       <c r="L117" t="s" s="2">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="M117" t="s" s="2">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="N117" t="s" s="2">
-        <v>341</v>
+        <v>342</v>
       </c>
       <c r="O117" t="s" s="2">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="P117" t="s" s="2">
         <v>78</v>
@@ -15607,7 +15610,7 @@
         <v>78</v>
       </c>
       <c r="AF117" t="s" s="2">
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="AG117" t="s" s="2">
         <v>79</v>
@@ -15622,10 +15625,10 @@
         <v>100</v>
       </c>
       <c r="AK117" t="s" s="2">
-        <v>344</v>
+        <v>345</v>
       </c>
       <c r="AL117" t="s" s="2">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="AM117" t="s" s="2">
         <v>78</v>
@@ -15636,10 +15639,10 @@
     </row>
     <row r="118">
       <c r="A118" t="s" s="2">
-        <v>489</v>
+        <v>490</v>
       </c>
       <c r="B118" t="s" s="2">
-        <v>451</v>
+        <v>452</v>
       </c>
       <c r="C118" s="2"/>
       <c r="D118" t="s" s="2">
@@ -15748,10 +15751,10 @@
     </row>
     <row r="119">
       <c r="A119" t="s" s="2">
-        <v>490</v>
+        <v>491</v>
       </c>
       <c r="B119" t="s" s="2">
-        <v>453</v>
+        <v>454</v>
       </c>
       <c r="C119" s="2"/>
       <c r="D119" t="s" s="2">
@@ -15862,10 +15865,10 @@
     </row>
     <row r="120">
       <c r="A120" t="s" s="2">
-        <v>491</v>
+        <v>492</v>
       </c>
       <c r="B120" t="s" s="2">
-        <v>455</v>
+        <v>456</v>
       </c>
       <c r="C120" s="2"/>
       <c r="D120" t="s" s="2">
@@ -15891,16 +15894,16 @@
         <v>130</v>
       </c>
       <c r="L120" t="s" s="2">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="M120" t="s" s="2">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="N120" t="s" s="2">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="O120" t="s" s="2">
-        <v>355</v>
+        <v>356</v>
       </c>
       <c r="P120" t="s" s="2">
         <v>78</v>
@@ -15949,7 +15952,7 @@
         <v>78</v>
       </c>
       <c r="AF120" t="s" s="2">
-        <v>357</v>
+        <v>358</v>
       </c>
       <c r="AG120" t="s" s="2">
         <v>79</v>
@@ -15964,10 +15967,10 @@
         <v>100</v>
       </c>
       <c r="AK120" t="s" s="2">
-        <v>358</v>
+        <v>359</v>
       </c>
       <c r="AL120" t="s" s="2">
-        <v>359</v>
+        <v>360</v>
       </c>
       <c r="AM120" t="s" s="2">
         <v>78</v>
@@ -15978,10 +15981,10 @@
     </row>
     <row r="121">
       <c r="A121" t="s" s="2">
-        <v>492</v>
+        <v>493</v>
       </c>
       <c r="B121" t="s" s="2">
-        <v>457</v>
+        <v>458</v>
       </c>
       <c r="C121" s="2"/>
       <c r="D121" t="s" s="2">
@@ -16007,13 +16010,13 @@
         <v>102</v>
       </c>
       <c r="L121" t="s" s="2">
-        <v>362</v>
+        <v>363</v>
       </c>
       <c r="M121" t="s" s="2">
-        <v>363</v>
+        <v>364</v>
       </c>
       <c r="N121" t="s" s="2">
-        <v>364</v>
+        <v>365</v>
       </c>
       <c r="O121" s="2"/>
       <c r="P121" t="s" s="2">
@@ -16063,7 +16066,7 @@
         <v>78</v>
       </c>
       <c r="AF121" t="s" s="2">
-        <v>365</v>
+        <v>366</v>
       </c>
       <c r="AG121" t="s" s="2">
         <v>79</v>
@@ -16078,10 +16081,10 @@
         <v>100</v>
       </c>
       <c r="AK121" t="s" s="2">
-        <v>366</v>
+        <v>367</v>
       </c>
       <c r="AL121" t="s" s="2">
-        <v>367</v>
+        <v>368</v>
       </c>
       <c r="AM121" t="s" s="2">
         <v>78</v>
@@ -16092,10 +16095,10 @@
     </row>
     <row r="122">
       <c r="A122" t="s" s="2">
-        <v>493</v>
+        <v>494</v>
       </c>
       <c r="B122" t="s" s="2">
-        <v>459</v>
+        <v>460</v>
       </c>
       <c r="C122" s="2"/>
       <c r="D122" t="s" s="2">
@@ -16121,14 +16124,14 @@
         <v>169</v>
       </c>
       <c r="L122" t="s" s="2">
-        <v>460</v>
+        <v>461</v>
       </c>
       <c r="M122" t="s" s="2">
-        <v>371</v>
+        <v>372</v>
       </c>
       <c r="N122" s="2"/>
       <c r="O122" t="s" s="2">
-        <v>372</v>
+        <v>373</v>
       </c>
       <c r="P122" t="s" s="2">
         <v>78</v>
@@ -16177,7 +16180,7 @@
         <v>78</v>
       </c>
       <c r="AF122" t="s" s="2">
-        <v>373</v>
+        <v>374</v>
       </c>
       <c r="AG122" t="s" s="2">
         <v>79</v>
@@ -16192,10 +16195,10 @@
         <v>100</v>
       </c>
       <c r="AK122" t="s" s="2">
-        <v>374</v>
+        <v>375</v>
       </c>
       <c r="AL122" t="s" s="2">
-        <v>375</v>
+        <v>376</v>
       </c>
       <c r="AM122" t="s" s="2">
         <v>78</v>
@@ -16206,10 +16209,10 @@
     </row>
     <row r="123">
       <c r="A123" t="s" s="2">
-        <v>494</v>
+        <v>495</v>
       </c>
       <c r="B123" t="s" s="2">
-        <v>462</v>
+        <v>463</v>
       </c>
       <c r="C123" s="2"/>
       <c r="D123" t="s" s="2">
@@ -16235,14 +16238,14 @@
         <v>102</v>
       </c>
       <c r="L123" t="s" s="2">
-        <v>378</v>
+        <v>379</v>
       </c>
       <c r="M123" t="s" s="2">
-        <v>379</v>
+        <v>380</v>
       </c>
       <c r="N123" s="2"/>
       <c r="O123" t="s" s="2">
-        <v>380</v>
+        <v>381</v>
       </c>
       <c r="P123" t="s" s="2">
         <v>78</v>
@@ -16291,7 +16294,7 @@
         <v>78</v>
       </c>
       <c r="AF123" t="s" s="2">
-        <v>381</v>
+        <v>382</v>
       </c>
       <c r="AG123" t="s" s="2">
         <v>79</v>
@@ -16306,10 +16309,10 @@
         <v>100</v>
       </c>
       <c r="AK123" t="s" s="2">
-        <v>382</v>
+        <v>383</v>
       </c>
       <c r="AL123" t="s" s="2">
-        <v>383</v>
+        <v>384</v>
       </c>
       <c r="AM123" t="s" s="2">
         <v>78</v>
@@ -16320,10 +16323,10 @@
     </row>
     <row r="124">
       <c r="A124" t="s" s="2">
-        <v>495</v>
+        <v>496</v>
       </c>
       <c r="B124" t="s" s="2">
-        <v>464</v>
+        <v>465</v>
       </c>
       <c r="C124" s="2"/>
       <c r="D124" t="s" s="2">
@@ -16346,19 +16349,19 @@
         <v>89</v>
       </c>
       <c r="K124" t="s" s="2">
-        <v>386</v>
+        <v>387</v>
       </c>
       <c r="L124" t="s" s="2">
-        <v>387</v>
+        <v>388</v>
       </c>
       <c r="M124" t="s" s="2">
-        <v>388</v>
+        <v>389</v>
       </c>
       <c r="N124" t="s" s="2">
-        <v>389</v>
+        <v>390</v>
       </c>
       <c r="O124" t="s" s="2">
-        <v>390</v>
+        <v>391</v>
       </c>
       <c r="P124" t="s" s="2">
         <v>78</v>
@@ -16407,7 +16410,7 @@
         <v>78</v>
       </c>
       <c r="AF124" t="s" s="2">
-        <v>391</v>
+        <v>392</v>
       </c>
       <c r="AG124" t="s" s="2">
         <v>79</v>
@@ -16422,10 +16425,10 @@
         <v>100</v>
       </c>
       <c r="AK124" t="s" s="2">
-        <v>392</v>
+        <v>393</v>
       </c>
       <c r="AL124" t="s" s="2">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="AM124" t="s" s="2">
         <v>78</v>
@@ -16436,10 +16439,10 @@
     </row>
     <row r="125">
       <c r="A125" t="s" s="2">
-        <v>496</v>
+        <v>497</v>
       </c>
       <c r="B125" t="s" s="2">
-        <v>466</v>
+        <v>467</v>
       </c>
       <c r="C125" s="2"/>
       <c r="D125" t="s" s="2">
@@ -16465,16 +16468,16 @@
         <v>102</v>
       </c>
       <c r="L125" t="s" s="2">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="M125" t="s" s="2">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="N125" t="s" s="2">
-        <v>398</v>
+        <v>399</v>
       </c>
       <c r="O125" t="s" s="2">
-        <v>399</v>
+        <v>400</v>
       </c>
       <c r="P125" t="s" s="2">
         <v>78</v>
@@ -16523,7 +16526,7 @@
         <v>78</v>
       </c>
       <c r="AF125" t="s" s="2">
-        <v>400</v>
+        <v>401</v>
       </c>
       <c r="AG125" t="s" s="2">
         <v>79</v>
@@ -16538,10 +16541,10 @@
         <v>100</v>
       </c>
       <c r="AK125" t="s" s="2">
-        <v>401</v>
+        <v>402</v>
       </c>
       <c r="AL125" t="s" s="2">
-        <v>402</v>
+        <v>403</v>
       </c>
       <c r="AM125" t="s" s="2">
         <v>78</v>
@@ -16552,10 +16555,10 @@
     </row>
     <row r="126">
       <c r="A126" t="s" s="2">
-        <v>497</v>
+        <v>498</v>
       </c>
       <c r="B126" t="s" s="2">
-        <v>497</v>
+        <v>498</v>
       </c>
       <c r="C126" s="2"/>
       <c r="D126" t="s" s="2">
@@ -16581,16 +16584,16 @@
         <v>102</v>
       </c>
       <c r="L126" t="s" s="2">
-        <v>498</v>
+        <v>499</v>
       </c>
       <c r="M126" t="s" s="2">
-        <v>499</v>
+        <v>500</v>
       </c>
       <c r="N126" t="s" s="2">
-        <v>500</v>
+        <v>501</v>
       </c>
       <c r="O126" t="s" s="2">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="P126" t="s" s="2">
         <v>78</v>
@@ -16639,7 +16642,7 @@
         <v>78</v>
       </c>
       <c r="AF126" t="s" s="2">
-        <v>497</v>
+        <v>498</v>
       </c>
       <c r="AG126" t="s" s="2">
         <v>79</v>
@@ -16654,13 +16657,13 @@
         <v>100</v>
       </c>
       <c r="AK126" t="s" s="2">
-        <v>502</v>
+        <v>503</v>
       </c>
       <c r="AL126" t="s" s="2">
-        <v>503</v>
+        <v>504</v>
       </c>
       <c r="AM126" t="s" s="2">
-        <v>504</v>
+        <v>505</v>
       </c>
       <c r="AN126" t="s" s="2">
         <v>78</v>
@@ -16668,10 +16671,10 @@
     </row>
     <row r="127">
       <c r="A127" t="s" s="2">
-        <v>505</v>
+        <v>506</v>
       </c>
       <c r="B127" t="s" s="2">
-        <v>505</v>
+        <v>506</v>
       </c>
       <c r="C127" s="2"/>
       <c r="D127" t="s" s="2">
@@ -16697,16 +16700,16 @@
         <v>102</v>
       </c>
       <c r="L127" t="s" s="2">
-        <v>506</v>
+        <v>507</v>
       </c>
       <c r="M127" t="s" s="2">
-        <v>507</v>
+        <v>508</v>
       </c>
       <c r="N127" t="s" s="2">
-        <v>508</v>
+        <v>509</v>
       </c>
       <c r="O127" t="s" s="2">
-        <v>509</v>
+        <v>510</v>
       </c>
       <c r="P127" t="s" s="2">
         <v>78</v>
@@ -16755,7 +16758,7 @@
         <v>78</v>
       </c>
       <c r="AF127" t="s" s="2">
-        <v>505</v>
+        <v>506</v>
       </c>
       <c r="AG127" t="s" s="2">
         <v>79</v>
@@ -16773,7 +16776,7 @@
         <v>78</v>
       </c>
       <c r="AL127" t="s" s="2">
-        <v>503</v>
+        <v>504</v>
       </c>
       <c r="AM127" t="s" s="2">
         <v>78</v>
@@ -16784,10 +16787,10 @@
     </row>
     <row r="128">
       <c r="A128" t="s" s="2">
-        <v>510</v>
+        <v>511</v>
       </c>
       <c r="B128" t="s" s="2">
-        <v>510</v>
+        <v>511</v>
       </c>
       <c r="C128" s="2"/>
       <c r="D128" t="s" s="2">
@@ -16810,19 +16813,19 @@
         <v>78</v>
       </c>
       <c r="K128" t="s" s="2">
-        <v>511</v>
+        <v>512</v>
       </c>
       <c r="L128" t="s" s="2">
-        <v>512</v>
+        <v>513</v>
       </c>
       <c r="M128" t="s" s="2">
-        <v>513</v>
+        <v>514</v>
       </c>
       <c r="N128" t="s" s="2">
-        <v>514</v>
+        <v>515</v>
       </c>
       <c r="O128" t="s" s="2">
-        <v>515</v>
+        <v>516</v>
       </c>
       <c r="P128" t="s" s="2">
         <v>78</v>
@@ -16871,7 +16874,7 @@
         <v>78</v>
       </c>
       <c r="AF128" t="s" s="2">
-        <v>510</v>
+        <v>511</v>
       </c>
       <c r="AG128" t="s" s="2">
         <v>79</v>
@@ -16880,19 +16883,19 @@
         <v>80</v>
       </c>
       <c r="AI128" t="s" s="2">
-        <v>516</v>
+        <v>517</v>
       </c>
       <c r="AJ128" t="s" s="2">
-        <v>517</v>
+        <v>518</v>
       </c>
       <c r="AK128" t="s" s="2">
-        <v>518</v>
+        <v>519</v>
       </c>
       <c r="AL128" t="s" s="2">
-        <v>519</v>
+        <v>520</v>
       </c>
       <c r="AM128" t="s" s="2">
-        <v>520</v>
+        <v>521</v>
       </c>
       <c r="AN128" t="s" s="2">
         <v>78</v>
@@ -16900,10 +16903,10 @@
     </row>
     <row r="129">
       <c r="A129" t="s" s="2">
-        <v>521</v>
+        <v>522</v>
       </c>
       <c r="B129" t="s" s="2">
-        <v>521</v>
+        <v>522</v>
       </c>
       <c r="C129" s="2"/>
       <c r="D129" t="s" s="2">
@@ -16926,19 +16929,19 @@
         <v>78</v>
       </c>
       <c r="K129" t="s" s="2">
-        <v>522</v>
+        <v>523</v>
       </c>
       <c r="L129" t="s" s="2">
-        <v>523</v>
+        <v>524</v>
       </c>
       <c r="M129" t="s" s="2">
-        <v>524</v>
+        <v>525</v>
       </c>
       <c r="N129" t="s" s="2">
-        <v>525</v>
+        <v>526</v>
       </c>
       <c r="O129" t="s" s="2">
-        <v>526</v>
+        <v>527</v>
       </c>
       <c r="P129" t="s" s="2">
         <v>78</v>
@@ -16987,7 +16990,7 @@
         <v>78</v>
       </c>
       <c r="AF129" t="s" s="2">
-        <v>521</v>
+        <v>522</v>
       </c>
       <c r="AG129" t="s" s="2">
         <v>79</v>
@@ -16996,19 +16999,19 @@
         <v>80</v>
       </c>
       <c r="AI129" t="s" s="2">
-        <v>527</v>
+        <v>528</v>
       </c>
       <c r="AJ129" t="s" s="2">
-        <v>528</v>
+        <v>529</v>
       </c>
       <c r="AK129" t="s" s="2">
-        <v>529</v>
+        <v>530</v>
       </c>
       <c r="AL129" t="s" s="2">
-        <v>530</v>
+        <v>531</v>
       </c>
       <c r="AM129" t="s" s="2">
-        <v>531</v>
+        <v>532</v>
       </c>
       <c r="AN129" t="s" s="2">
         <v>78</v>
@@ -17016,10 +17019,10 @@
     </row>
     <row r="130">
       <c r="A130" t="s" s="2">
-        <v>532</v>
+        <v>533</v>
       </c>
       <c r="B130" t="s" s="2">
-        <v>532</v>
+        <v>533</v>
       </c>
       <c r="C130" s="2"/>
       <c r="D130" t="s" s="2">
@@ -17042,17 +17045,17 @@
         <v>89</v>
       </c>
       <c r="K130" t="s" s="2">
-        <v>533</v>
+        <v>534</v>
       </c>
       <c r="L130" t="s" s="2">
-        <v>534</v>
+        <v>535</v>
       </c>
       <c r="M130" t="s" s="2">
-        <v>535</v>
+        <v>536</v>
       </c>
       <c r="N130" s="2"/>
       <c r="O130" t="s" s="2">
-        <v>536</v>
+        <v>537</v>
       </c>
       <c r="P130" t="s" s="2">
         <v>78</v>
@@ -17101,7 +17104,7 @@
         <v>78</v>
       </c>
       <c r="AF130" t="s" s="2">
-        <v>532</v>
+        <v>533</v>
       </c>
       <c r="AG130" t="s" s="2">
         <v>79</v>
@@ -17116,10 +17119,10 @@
         <v>100</v>
       </c>
       <c r="AK130" t="s" s="2">
-        <v>427</v>
+        <v>428</v>
       </c>
       <c r="AL130" t="s" s="2">
-        <v>537</v>
+        <v>538</v>
       </c>
       <c r="AM130" t="s" s="2">
         <v>106</v>
@@ -17130,10 +17133,10 @@
     </row>
     <row r="131">
       <c r="A131" t="s" s="2">
-        <v>538</v>
+        <v>539</v>
       </c>
       <c r="B131" t="s" s="2">
-        <v>538</v>
+        <v>539</v>
       </c>
       <c r="C131" s="2"/>
       <c r="D131" t="s" s="2">
@@ -17242,10 +17245,10 @@
     </row>
     <row r="132">
       <c r="A132" t="s" s="2">
-        <v>539</v>
+        <v>540</v>
       </c>
       <c r="B132" t="s" s="2">
-        <v>539</v>
+        <v>540</v>
       </c>
       <c r="C132" s="2"/>
       <c r="D132" t="s" s="2">
@@ -17356,10 +17359,10 @@
     </row>
     <row r="133">
       <c r="A133" t="s" s="2">
-        <v>540</v>
+        <v>541</v>
       </c>
       <c r="B133" t="s" s="2">
-        <v>540</v>
+        <v>541</v>
       </c>
       <c r="C133" s="2"/>
       <c r="D133" t="s" s="2">
@@ -17385,13 +17388,13 @@
         <v>102</v>
       </c>
       <c r="L133" t="s" s="2">
-        <v>541</v>
+        <v>542</v>
       </c>
       <c r="M133" t="s" s="2">
-        <v>542</v>
+        <v>543</v>
       </c>
       <c r="N133" t="s" s="2">
-        <v>543</v>
+        <v>544</v>
       </c>
       <c r="O133" s="2"/>
       <c r="P133" t="s" s="2">
@@ -17441,7 +17444,7 @@
         <v>78</v>
       </c>
       <c r="AF133" t="s" s="2">
-        <v>544</v>
+        <v>545</v>
       </c>
       <c r="AG133" t="s" s="2">
         <v>79</v>
@@ -17450,7 +17453,7 @@
         <v>88</v>
       </c>
       <c r="AI133" t="s" s="2">
-        <v>545</v>
+        <v>546</v>
       </c>
       <c r="AJ133" t="s" s="2">
         <v>100</v>
@@ -17470,10 +17473,10 @@
     </row>
     <row r="134">
       <c r="A134" t="s" s="2">
-        <v>546</v>
+        <v>547</v>
       </c>
       <c r="B134" t="s" s="2">
-        <v>546</v>
+        <v>547</v>
       </c>
       <c r="C134" s="2"/>
       <c r="D134" t="s" s="2">
@@ -17499,13 +17502,13 @@
         <v>130</v>
       </c>
       <c r="L134" t="s" s="2">
-        <v>547</v>
+        <v>548</v>
       </c>
       <c r="M134" t="s" s="2">
-        <v>548</v>
+        <v>549</v>
       </c>
       <c r="N134" t="s" s="2">
-        <v>549</v>
+        <v>550</v>
       </c>
       <c r="O134" s="2"/>
       <c r="P134" t="s" s="2">
@@ -17535,7 +17538,7 @@
       </c>
       <c r="Y134" s="2"/>
       <c r="Z134" t="s" s="2">
-        <v>443</v>
+        <v>444</v>
       </c>
       <c r="AA134" t="s" s="2">
         <v>78</v>
@@ -17553,7 +17556,7 @@
         <v>78</v>
       </c>
       <c r="AF134" t="s" s="2">
-        <v>550</v>
+        <v>551</v>
       </c>
       <c r="AG134" t="s" s="2">
         <v>79</v>
@@ -17582,10 +17585,10 @@
     </row>
     <row r="135">
       <c r="A135" t="s" s="2">
-        <v>551</v>
+        <v>552</v>
       </c>
       <c r="B135" t="s" s="2">
-        <v>551</v>
+        <v>552</v>
       </c>
       <c r="C135" s="2"/>
       <c r="D135" t="s" s="2">
@@ -17611,13 +17614,13 @@
         <v>218</v>
       </c>
       <c r="L135" t="s" s="2">
-        <v>552</v>
+        <v>553</v>
       </c>
       <c r="M135" t="s" s="2">
-        <v>553</v>
+        <v>554</v>
       </c>
       <c r="N135" t="s" s="2">
-        <v>554</v>
+        <v>555</v>
       </c>
       <c r="O135" s="2"/>
       <c r="P135" t="s" s="2">
@@ -17667,7 +17670,7 @@
         <v>78</v>
       </c>
       <c r="AF135" t="s" s="2">
-        <v>555</v>
+        <v>556</v>
       </c>
       <c r="AG135" t="s" s="2">
         <v>79</v>
@@ -17685,7 +17688,7 @@
         <v>78</v>
       </c>
       <c r="AL135" t="s" s="2">
-        <v>556</v>
+        <v>557</v>
       </c>
       <c r="AM135" t="s" s="2">
         <v>78</v>
@@ -17696,10 +17699,10 @@
     </row>
     <row r="136">
       <c r="A136" t="s" s="2">
-        <v>557</v>
+        <v>558</v>
       </c>
       <c r="B136" t="s" s="2">
-        <v>557</v>
+        <v>558</v>
       </c>
       <c r="C136" s="2"/>
       <c r="D136" t="s" s="2">
@@ -17725,13 +17728,13 @@
         <v>102</v>
       </c>
       <c r="L136" t="s" s="2">
-        <v>558</v>
+        <v>559</v>
       </c>
       <c r="M136" t="s" s="2">
-        <v>559</v>
+        <v>560</v>
       </c>
       <c r="N136" t="s" s="2">
-        <v>560</v>
+        <v>561</v>
       </c>
       <c r="O136" s="2"/>
       <c r="P136" t="s" s="2">
@@ -17781,7 +17784,7 @@
         <v>78</v>
       </c>
       <c r="AF136" t="s" s="2">
-        <v>561</v>
+        <v>562</v>
       </c>
       <c r="AG136" t="s" s="2">
         <v>79</v>
@@ -17810,10 +17813,10 @@
     </row>
     <row r="137">
       <c r="A137" t="s" s="2">
-        <v>562</v>
+        <v>563</v>
       </c>
       <c r="B137" t="s" s="2">
-        <v>562</v>
+        <v>563</v>
       </c>
       <c r="C137" s="2"/>
       <c r="D137" t="s" s="2">
@@ -17836,19 +17839,19 @@
         <v>78</v>
       </c>
       <c r="K137" t="s" s="2">
-        <v>563</v>
+        <v>564</v>
       </c>
       <c r="L137" t="s" s="2">
-        <v>564</v>
+        <v>565</v>
       </c>
       <c r="M137" t="s" s="2">
-        <v>565</v>
+        <v>566</v>
       </c>
       <c r="N137" t="s" s="2">
-        <v>566</v>
+        <v>567</v>
       </c>
       <c r="O137" t="s" s="2">
-        <v>567</v>
+        <v>568</v>
       </c>
       <c r="P137" t="s" s="2">
         <v>78</v>
@@ -17897,7 +17900,7 @@
         <v>78</v>
       </c>
       <c r="AF137" t="s" s="2">
-        <v>562</v>
+        <v>563</v>
       </c>
       <c r="AG137" t="s" s="2">
         <v>79</v>
@@ -17915,7 +17918,7 @@
         <v>78</v>
       </c>
       <c r="AL137" t="s" s="2">
-        <v>568</v>
+        <v>569</v>
       </c>
       <c r="AM137" t="s" s="2">
         <v>78</v>
@@ -17926,10 +17929,10 @@
     </row>
     <row r="138">
       <c r="A138" t="s" s="2">
-        <v>569</v>
+        <v>570</v>
       </c>
       <c r="B138" t="s" s="2">
-        <v>569</v>
+        <v>570</v>
       </c>
       <c r="C138" s="2"/>
       <c r="D138" t="s" s="2">
@@ -18038,10 +18041,10 @@
     </row>
     <row r="139">
       <c r="A139" t="s" s="2">
-        <v>570</v>
+        <v>571</v>
       </c>
       <c r="B139" t="s" s="2">
-        <v>570</v>
+        <v>571</v>
       </c>
       <c r="C139" s="2"/>
       <c r="D139" t="s" s="2">
@@ -18152,14 +18155,14 @@
     </row>
     <row r="140">
       <c r="A140" t="s" s="2">
-        <v>571</v>
+        <v>572</v>
       </c>
       <c r="B140" t="s" s="2">
-        <v>571</v>
+        <v>572</v>
       </c>
       <c r="C140" s="2"/>
       <c r="D140" t="s" s="2">
-        <v>572</v>
+        <v>573</v>
       </c>
       <c r="E140" s="2"/>
       <c r="F140" t="s" s="2">
@@ -18181,10 +18184,10 @@
         <v>109</v>
       </c>
       <c r="L140" t="s" s="2">
-        <v>573</v>
+        <v>574</v>
       </c>
       <c r="M140" t="s" s="2">
-        <v>574</v>
+        <v>575</v>
       </c>
       <c r="N140" t="s" s="2">
         <v>112</v>
@@ -18239,7 +18242,7 @@
         <v>78</v>
       </c>
       <c r="AF140" t="s" s="2">
-        <v>575</v>
+        <v>576</v>
       </c>
       <c r="AG140" t="s" s="2">
         <v>79</v>
@@ -18268,10 +18271,10 @@
     </row>
     <row r="141">
       <c r="A141" t="s" s="2">
-        <v>576</v>
+        <v>577</v>
       </c>
       <c r="B141" t="s" s="2">
-        <v>576</v>
+        <v>577</v>
       </c>
       <c r="C141" s="2"/>
       <c r="D141" t="s" s="2">
@@ -18297,14 +18300,14 @@
         <v>241</v>
       </c>
       <c r="L141" t="s" s="2">
-        <v>577</v>
+        <v>578</v>
       </c>
       <c r="M141" t="s" s="2">
-        <v>578</v>
+        <v>579</v>
       </c>
       <c r="N141" s="2"/>
       <c r="O141" t="s" s="2">
-        <v>579</v>
+        <v>580</v>
       </c>
       <c r="P141" t="s" s="2">
         <v>78</v>
@@ -18332,10 +18335,10 @@
         <v>151</v>
       </c>
       <c r="Y141" t="s" s="2">
-        <v>580</v>
+        <v>581</v>
       </c>
       <c r="Z141" t="s" s="2">
-        <v>581</v>
+        <v>582</v>
       </c>
       <c r="AA141" t="s" s="2">
         <v>78</v>
@@ -18353,7 +18356,7 @@
         <v>78</v>
       </c>
       <c r="AF141" t="s" s="2">
-        <v>576</v>
+        <v>577</v>
       </c>
       <c r="AG141" t="s" s="2">
         <v>79</v>
@@ -18371,7 +18374,7 @@
         <v>78</v>
       </c>
       <c r="AL141" t="s" s="2">
-        <v>582</v>
+        <v>583</v>
       </c>
       <c r="AM141" t="s" s="2">
         <v>78</v>
@@ -18382,10 +18385,10 @@
     </row>
     <row r="142">
       <c r="A142" t="s" s="2">
-        <v>583</v>
+        <v>584</v>
       </c>
       <c r="B142" t="s" s="2">
-        <v>583</v>
+        <v>584</v>
       </c>
       <c r="C142" s="2"/>
       <c r="D142" t="s" s="2">
@@ -18408,17 +18411,17 @@
         <v>78</v>
       </c>
       <c r="K142" t="s" s="2">
-        <v>584</v>
+        <v>585</v>
       </c>
       <c r="L142" t="s" s="2">
-        <v>585</v>
+        <v>586</v>
       </c>
       <c r="M142" t="s" s="2">
-        <v>586</v>
+        <v>587</v>
       </c>
       <c r="N142" s="2"/>
       <c r="O142" t="s" s="2">
-        <v>587</v>
+        <v>588</v>
       </c>
       <c r="P142" t="s" s="2">
         <v>78</v>
@@ -18467,7 +18470,7 @@
         <v>78</v>
       </c>
       <c r="AF142" t="s" s="2">
-        <v>583</v>
+        <v>584</v>
       </c>
       <c r="AG142" t="s" s="2">
         <v>79</v>
@@ -18482,10 +18485,10 @@
         <v>100</v>
       </c>
       <c r="AK142" t="s" s="2">
-        <v>588</v>
+        <v>589</v>
       </c>
       <c r="AL142" t="s" s="2">
-        <v>589</v>
+        <v>590</v>
       </c>
       <c r="AM142" t="s" s="2">
         <v>78</v>
@@ -18496,10 +18499,10 @@
     </row>
     <row r="143">
       <c r="A143" t="s" s="2">
-        <v>590</v>
+        <v>591</v>
       </c>
       <c r="B143" t="s" s="2">
-        <v>590</v>
+        <v>591</v>
       </c>
       <c r="C143" s="2"/>
       <c r="D143" t="s" s="2">
@@ -18522,17 +18525,17 @@
         <v>78</v>
       </c>
       <c r="K143" t="s" s="2">
-        <v>511</v>
+        <v>512</v>
       </c>
       <c r="L143" t="s" s="2">
-        <v>591</v>
+        <v>592</v>
       </c>
       <c r="M143" t="s" s="2">
-        <v>592</v>
+        <v>593</v>
       </c>
       <c r="N143" s="2"/>
       <c r="O143" t="s" s="2">
-        <v>593</v>
+        <v>594</v>
       </c>
       <c r="P143" t="s" s="2">
         <v>78</v>
@@ -18581,7 +18584,7 @@
         <v>78</v>
       </c>
       <c r="AF143" t="s" s="2">
-        <v>590</v>
+        <v>591</v>
       </c>
       <c r="AG143" t="s" s="2">
         <v>79</v>
@@ -18596,10 +18599,10 @@
         <v>100</v>
       </c>
       <c r="AK143" t="s" s="2">
-        <v>594</v>
+        <v>595</v>
       </c>
       <c r="AL143" t="s" s="2">
-        <v>595</v>
+        <v>596</v>
       </c>
       <c r="AM143" t="s" s="2">
         <v>78</v>
@@ -18610,10 +18613,10 @@
     </row>
     <row r="144">
       <c r="A144" t="s" s="2">
-        <v>596</v>
+        <v>597</v>
       </c>
       <c r="B144" t="s" s="2">
-        <v>596</v>
+        <v>597</v>
       </c>
       <c r="C144" s="2"/>
       <c r="D144" t="s" s="2">
@@ -18636,17 +18639,17 @@
         <v>78</v>
       </c>
       <c r="K144" t="s" s="2">
-        <v>522</v>
+        <v>523</v>
       </c>
       <c r="L144" t="s" s="2">
-        <v>597</v>
+        <v>598</v>
       </c>
       <c r="M144" t="s" s="2">
-        <v>598</v>
+        <v>599</v>
       </c>
       <c r="N144" s="2"/>
       <c r="O144" t="s" s="2">
-        <v>599</v>
+        <v>600</v>
       </c>
       <c r="P144" t="s" s="2">
         <v>78</v>
@@ -18695,7 +18698,7 @@
         <v>78</v>
       </c>
       <c r="AF144" t="s" s="2">
-        <v>596</v>
+        <v>597</v>
       </c>
       <c r="AG144" t="s" s="2">
         <v>79</v>
@@ -18710,10 +18713,10 @@
         <v>100</v>
       </c>
       <c r="AK144" t="s" s="2">
-        <v>600</v>
+        <v>601</v>
       </c>
       <c r="AL144" t="s" s="2">
-        <v>601</v>
+        <v>602</v>
       </c>
       <c r="AM144" t="s" s="2">
         <v>78</v>
@@ -18724,10 +18727,10 @@
     </row>
     <row r="145">
       <c r="A145" t="s" s="2">
-        <v>602</v>
+        <v>603</v>
       </c>
       <c r="B145" t="s" s="2">
-        <v>602</v>
+        <v>603</v>
       </c>
       <c r="C145" s="2"/>
       <c r="D145" t="s" s="2">
@@ -18750,17 +18753,17 @@
         <v>78</v>
       </c>
       <c r="K145" t="s" s="2">
-        <v>603</v>
+        <v>604</v>
       </c>
       <c r="L145" t="s" s="2">
-        <v>604</v>
+        <v>605</v>
       </c>
       <c r="M145" t="s" s="2">
-        <v>605</v>
+        <v>606</v>
       </c>
       <c r="N145" s="2"/>
       <c r="O145" t="s" s="2">
-        <v>606</v>
+        <v>607</v>
       </c>
       <c r="P145" t="s" s="2">
         <v>78</v>
@@ -18809,7 +18812,7 @@
         <v>78</v>
       </c>
       <c r="AF145" t="s" s="2">
-        <v>602</v>
+        <v>603</v>
       </c>
       <c r="AG145" t="s" s="2">
         <v>79</v>

</xml_diff>